<commit_message>
excel pernoctaciones por dia
</commit_message>
<xml_diff>
--- a/EDA/DF_DV/Pernoctaciones por dias.xlsx
+++ b/EDA/DF_DV/Pernoctaciones por dias.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,9 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -425,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F144"/>
+  <dimension ref="A1:F142"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,10 +467,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>2011-01</t>
-        </is>
+      <c r="A2" s="2" t="n">
+        <v>40544</v>
       </c>
       <c r="B2" t="n">
         <v>120035</v>
@@ -483,10 +487,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>2011-02</t>
-        </is>
+      <c r="A3" s="2" t="n">
+        <v>40575</v>
       </c>
       <c r="B3" t="n">
         <v>140090</v>
@@ -505,10 +507,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>2011-03</t>
-        </is>
+      <c r="A4" s="2" t="n">
+        <v>40603</v>
       </c>
       <c r="B4" t="n">
         <v>177734</v>
@@ -527,10 +527,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>2011-04</t>
-        </is>
+      <c r="A5" s="2" t="n">
+        <v>40634</v>
       </c>
       <c r="B5" t="n">
         <v>218319</v>
@@ -549,10 +547,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>2011-05</t>
-        </is>
+      <c r="A6" s="2" t="n">
+        <v>40664</v>
       </c>
       <c r="B6" t="n">
         <v>207706</v>
@@ -571,10 +567,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>2011-06</t>
-        </is>
+      <c r="A7" s="2" t="n">
+        <v>40695</v>
       </c>
       <c r="B7" t="n">
         <v>225072</v>
@@ -593,10 +587,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>2011-07</t>
-        </is>
+      <c r="A8" s="2" t="n">
+        <v>40725</v>
       </c>
       <c r="B8" t="n">
         <v>273814</v>
@@ -615,10 +607,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>2011-08</t>
-        </is>
+      <c r="A9" s="2" t="n">
+        <v>40756</v>
       </c>
       <c r="B9" t="n">
         <v>277775</v>
@@ -637,10 +627,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>2011-09</t>
-        </is>
+      <c r="A10" s="2" t="n">
+        <v>40787</v>
       </c>
       <c r="B10" t="n">
         <v>239742</v>
@@ -659,10 +647,8 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>2011-10</t>
-        </is>
+      <c r="A11" s="2" t="n">
+        <v>40817</v>
       </c>
       <c r="B11" t="n">
         <v>217931</v>
@@ -681,10 +667,8 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>2011-11</t>
-        </is>
+      <c r="A12" s="2" t="n">
+        <v>40848</v>
       </c>
       <c r="B12" t="n">
         <v>165304</v>
@@ -703,10 +687,8 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="inlineStr">
-        <is>
-          <t>2011-12</t>
-        </is>
+      <c r="A13" s="2" t="n">
+        <v>40878</v>
       </c>
       <c r="B13" t="n">
         <v>157475</v>
@@ -725,10 +707,8 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="inlineStr">
-        <is>
-          <t>2012-01</t>
-        </is>
+      <c r="A14" s="2" t="n">
+        <v>40909</v>
       </c>
       <c r="B14" t="n">
         <v>126707</v>
@@ -747,10 +727,8 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="inlineStr">
-        <is>
-          <t>2012-02</t>
-        </is>
+      <c r="A15" s="2" t="n">
+        <v>40940</v>
       </c>
       <c r="B15" t="n">
         <v>135134</v>
@@ -769,10 +747,8 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="inlineStr">
-        <is>
-          <t>2012-03</t>
-        </is>
+      <c r="A16" s="2" t="n">
+        <v>40969</v>
       </c>
       <c r="B16" t="n">
         <v>183929</v>
@@ -791,10 +767,8 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="inlineStr">
-        <is>
-          <t>2012-04</t>
-        </is>
+      <c r="A17" s="2" t="n">
+        <v>41000</v>
       </c>
       <c r="B17" t="n">
         <v>204132</v>
@@ -813,10 +787,8 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="inlineStr">
-        <is>
-          <t>2012-05</t>
-        </is>
+      <c r="A18" s="2" t="n">
+        <v>41030</v>
       </c>
       <c r="B18" t="n">
         <v>217187</v>
@@ -835,10 +807,8 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="inlineStr">
-        <is>
-          <t>2012-06</t>
-        </is>
+      <c r="A19" s="2" t="n">
+        <v>41061</v>
       </c>
       <c r="B19" t="n">
         <v>228950</v>
@@ -857,10 +827,8 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="inlineStr">
-        <is>
-          <t>2012-07</t>
-        </is>
+      <c r="A20" s="2" t="n">
+        <v>41091</v>
       </c>
       <c r="B20" t="n">
         <v>263536</v>
@@ -879,10 +847,8 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="inlineStr">
-        <is>
-          <t>2012-08</t>
-        </is>
+      <c r="A21" s="2" t="n">
+        <v>41122</v>
       </c>
       <c r="B21" t="n">
         <v>287681</v>
@@ -901,10 +867,8 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="inlineStr">
-        <is>
-          <t>2012-09</t>
-        </is>
+      <c r="A22" s="2" t="n">
+        <v>41153</v>
       </c>
       <c r="B22" t="n">
         <v>237516</v>
@@ -923,10 +887,8 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="inlineStr">
-        <is>
-          <t>2012-10</t>
-        </is>
+      <c r="A23" s="2" t="n">
+        <v>41183</v>
       </c>
       <c r="B23" t="n">
         <v>210166</v>
@@ -945,10 +907,8 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="inlineStr">
-        <is>
-          <t>2012-11</t>
-        </is>
+      <c r="A24" s="2" t="n">
+        <v>41214</v>
       </c>
       <c r="B24" t="n">
         <v>172445</v>
@@ -967,10 +927,8 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="inlineStr">
-        <is>
-          <t>2012-12</t>
-        </is>
+      <c r="A25" s="2" t="n">
+        <v>41244</v>
       </c>
       <c r="B25" t="n">
         <v>152724</v>
@@ -989,10 +947,8 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="inlineStr">
-        <is>
-          <t>2013-01</t>
-        </is>
+      <c r="A26" s="2" t="n">
+        <v>41275</v>
       </c>
       <c r="B26" t="n">
         <v>121313</v>
@@ -1011,10 +967,8 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="inlineStr">
-        <is>
-          <t>2013-02</t>
-        </is>
+      <c r="A27" s="2" t="n">
+        <v>41306</v>
       </c>
       <c r="B27" t="n">
         <v>127728</v>
@@ -1033,10 +987,8 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="inlineStr">
-        <is>
-          <t>2013-03</t>
-        </is>
+      <c r="A28" s="2" t="n">
+        <v>41334</v>
       </c>
       <c r="B28" t="n">
         <v>186480</v>
@@ -1055,10 +1007,8 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="1" t="inlineStr">
-        <is>
-          <t>2013-04</t>
-        </is>
+      <c r="A29" s="2" t="n">
+        <v>41365</v>
       </c>
       <c r="B29" t="n">
         <v>174978</v>
@@ -1077,10 +1027,8 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="1" t="inlineStr">
-        <is>
-          <t>2013-05</t>
-        </is>
+      <c r="A30" s="2" t="n">
+        <v>41395</v>
       </c>
       <c r="B30" t="n">
         <v>221128</v>
@@ -1099,10 +1047,8 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="inlineStr">
-        <is>
-          <t>2013-06</t>
-        </is>
+      <c r="A31" s="2" t="n">
+        <v>41426</v>
       </c>
       <c r="B31" t="n">
         <v>213242</v>
@@ -1121,10 +1067,8 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="inlineStr">
-        <is>
-          <t>2013-07</t>
-        </is>
+      <c r="A32" s="2" t="n">
+        <v>41456</v>
       </c>
       <c r="B32" t="n">
         <v>260235</v>
@@ -1143,10 +1087,8 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="1" t="inlineStr">
-        <is>
-          <t>2013-08</t>
-        </is>
+      <c r="A33" s="2" t="n">
+        <v>41487</v>
       </c>
       <c r="B33" t="n">
         <v>294753</v>
@@ -1165,10 +1107,8 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="1" t="inlineStr">
-        <is>
-          <t>2013-09</t>
-        </is>
+      <c r="A34" s="2" t="n">
+        <v>41518</v>
       </c>
       <c r="B34" t="n">
         <v>235777</v>
@@ -1187,10 +1127,8 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="1" t="inlineStr">
-        <is>
-          <t>2013-10</t>
-        </is>
+      <c r="A35" s="2" t="n">
+        <v>41548</v>
       </c>
       <c r="B35" t="n">
         <v>211156</v>
@@ -1209,10 +1147,8 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="1" t="inlineStr">
-        <is>
-          <t>2013-11</t>
-        </is>
+      <c r="A36" s="2" t="n">
+        <v>41579</v>
       </c>
       <c r="B36" t="n">
         <v>170382</v>
@@ -1231,10 +1167,8 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="1" t="inlineStr">
-        <is>
-          <t>2013-12</t>
-        </is>
+      <c r="A37" s="2" t="n">
+        <v>41609</v>
       </c>
       <c r="B37" t="n">
         <v>150908</v>
@@ -1253,10 +1187,8 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="1" t="inlineStr">
-        <is>
-          <t>2014-01</t>
-        </is>
+      <c r="A38" s="2" t="n">
+        <v>41640</v>
       </c>
       <c r="B38" t="n">
         <v>114653</v>
@@ -1275,10 +1207,8 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="1" t="inlineStr">
-        <is>
-          <t>2014-02</t>
-        </is>
+      <c r="A39" s="2" t="n">
+        <v>41671</v>
       </c>
       <c r="B39" t="n">
         <v>128606</v>
@@ -1297,10 +1227,8 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="1" t="inlineStr">
-        <is>
-          <t>2014-03</t>
-        </is>
+      <c r="A40" s="2" t="n">
+        <v>41699</v>
       </c>
       <c r="B40" t="n">
         <v>161426</v>
@@ -1319,10 +1247,8 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="1" t="inlineStr">
-        <is>
-          <t>2014-04</t>
-        </is>
+      <c r="A41" s="2" t="n">
+        <v>41730</v>
       </c>
       <c r="B41" t="n">
         <v>188304</v>
@@ -1341,10 +1267,8 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="1" t="inlineStr">
-        <is>
-          <t>2014-05</t>
-        </is>
+      <c r="A42" s="2" t="n">
+        <v>41760</v>
       </c>
       <c r="B42" t="n">
         <v>229813</v>
@@ -1363,10 +1287,8 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="1" t="inlineStr">
-        <is>
-          <t>2014-06</t>
-        </is>
+      <c r="A43" s="2" t="n">
+        <v>41791</v>
       </c>
       <c r="B43" t="n">
         <v>226899</v>
@@ -1385,10 +1307,8 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="1" t="inlineStr">
-        <is>
-          <t>2014-07</t>
-        </is>
+      <c r="A44" s="2" t="n">
+        <v>41821</v>
       </c>
       <c r="B44" t="n">
         <v>261168</v>
@@ -1407,10 +1327,8 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="1" t="inlineStr">
-        <is>
-          <t>2014-08</t>
-        </is>
+      <c r="A45" s="2" t="n">
+        <v>41852</v>
       </c>
       <c r="B45" t="n">
         <v>308692</v>
@@ -1429,10 +1347,8 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="1" t="inlineStr">
-        <is>
-          <t>2014-09</t>
-        </is>
+      <c r="A46" s="2" t="n">
+        <v>41883</v>
       </c>
       <c r="B46" t="n">
         <v>239029</v>
@@ -1451,10 +1367,8 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="1" t="inlineStr">
-        <is>
-          <t>2014-10</t>
-        </is>
+      <c r="A47" s="2" t="n">
+        <v>41913</v>
       </c>
       <c r="B47" t="n">
         <v>229667</v>
@@ -1473,10 +1387,8 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="1" t="inlineStr">
-        <is>
-          <t>2014-11</t>
-        </is>
+      <c r="A48" s="2" t="n">
+        <v>41944</v>
       </c>
       <c r="B48" t="n">
         <v>176349</v>
@@ -1495,10 +1407,8 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="1" t="inlineStr">
-        <is>
-          <t>2014-12</t>
-        </is>
+      <c r="A49" s="2" t="n">
+        <v>41974</v>
       </c>
       <c r="B49" t="n">
         <v>160226</v>
@@ -1517,10 +1427,8 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="1" t="inlineStr">
-        <is>
-          <t>2015-01</t>
-        </is>
+      <c r="A50" s="2" t="n">
+        <v>42005</v>
       </c>
       <c r="B50" t="n">
         <v>125784</v>
@@ -1539,10 +1447,8 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="1" t="inlineStr">
-        <is>
-          <t>2015-02</t>
-        </is>
+      <c r="A51" s="2" t="n">
+        <v>42036</v>
       </c>
       <c r="B51" t="n">
         <v>136273</v>
@@ -1561,10 +1467,8 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="1" t="inlineStr">
-        <is>
-          <t>2015-03</t>
-        </is>
+      <c r="A52" s="2" t="n">
+        <v>42064</v>
       </c>
       <c r="B52" t="n">
         <v>175546</v>
@@ -1583,10 +1487,8 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="1" t="inlineStr">
-        <is>
-          <t>2015-04</t>
-        </is>
+      <c r="A53" s="2" t="n">
+        <v>42095</v>
       </c>
       <c r="B53" t="n">
         <v>208825</v>
@@ -1605,10 +1507,8 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="1" t="inlineStr">
-        <is>
-          <t>2015-05</t>
-        </is>
+      <c r="A54" s="2" t="n">
+        <v>42125</v>
       </c>
       <c r="B54" t="n">
         <v>244600</v>
@@ -1627,10 +1527,8 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="1" t="inlineStr">
-        <is>
-          <t>2015-06</t>
-        </is>
+      <c r="A55" s="2" t="n">
+        <v>42156</v>
       </c>
       <c r="B55" t="n">
         <v>242380</v>
@@ -1649,10 +1547,8 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="1" t="inlineStr">
-        <is>
-          <t>2015-07</t>
-        </is>
+      <c r="A56" s="2" t="n">
+        <v>42186</v>
       </c>
       <c r="B56" t="n">
         <v>293712</v>
@@ -1671,10 +1567,8 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="1" t="inlineStr">
-        <is>
-          <t>2015-08</t>
-        </is>
+      <c r="A57" s="2" t="n">
+        <v>42217</v>
       </c>
       <c r="B57" t="n">
         <v>322153</v>
@@ -1693,10 +1587,8 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="1" t="inlineStr">
-        <is>
-          <t>2015-09</t>
-        </is>
+      <c r="A58" s="2" t="n">
+        <v>42248</v>
       </c>
       <c r="B58" t="n">
         <v>262504</v>
@@ -1715,10 +1607,8 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="1" t="inlineStr">
-        <is>
-          <t>2015-10</t>
-        </is>
+      <c r="A59" s="2" t="n">
+        <v>42278</v>
       </c>
       <c r="B59" t="n">
         <v>255487</v>
@@ -1737,10 +1627,8 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="1" t="inlineStr">
-        <is>
-          <t>2015-11</t>
-        </is>
+      <c r="A60" s="2" t="n">
+        <v>42309</v>
       </c>
       <c r="B60" t="n">
         <v>185845</v>
@@ -1759,10 +1647,8 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="1" t="inlineStr">
-        <is>
-          <t>2015-12</t>
-        </is>
+      <c r="A61" s="2" t="n">
+        <v>42339</v>
       </c>
       <c r="B61" t="n">
         <v>184276</v>
@@ -1781,10 +1667,8 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="1" t="inlineStr">
-        <is>
-          <t>2016-01</t>
-        </is>
+      <c r="A62" s="2" t="n">
+        <v>42370</v>
       </c>
       <c r="B62" t="n">
         <v>141785</v>
@@ -1803,10 +1687,8 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="1" t="inlineStr">
-        <is>
-          <t>2016-02</t>
-        </is>
+      <c r="A63" s="2" t="n">
+        <v>42401</v>
       </c>
       <c r="B63" t="n">
         <v>162340</v>
@@ -1825,10 +1707,8 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="1" t="inlineStr">
-        <is>
-          <t>2016-03</t>
-        </is>
+      <c r="A64" s="2" t="n">
+        <v>42430</v>
       </c>
       <c r="B64" t="n">
         <v>208235</v>
@@ -1847,10 +1727,8 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="1" t="inlineStr">
-        <is>
-          <t>2016-04</t>
-        </is>
+      <c r="A65" s="2" t="n">
+        <v>42461</v>
       </c>
       <c r="B65" t="n">
         <v>221555</v>
@@ -1869,10 +1747,8 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="1" t="inlineStr">
-        <is>
-          <t>2016-05</t>
-        </is>
+      <c r="A66" s="2" t="n">
+        <v>42491</v>
       </c>
       <c r="B66" t="n">
         <v>260619</v>
@@ -1891,10 +1767,8 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="1" t="inlineStr">
-        <is>
-          <t>2016-06</t>
-        </is>
+      <c r="A67" s="2" t="n">
+        <v>42522</v>
       </c>
       <c r="B67" t="n">
         <v>257880</v>
@@ -1913,10 +1787,8 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="1" t="inlineStr">
-        <is>
-          <t>2016-07</t>
-        </is>
+      <c r="A68" s="2" t="n">
+        <v>42552</v>
       </c>
       <c r="B68" t="n">
         <v>313724</v>
@@ -1935,10 +1807,8 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="1" t="inlineStr">
-        <is>
-          <t>2016-08</t>
-        </is>
+      <c r="A69" s="2" t="n">
+        <v>42583</v>
       </c>
       <c r="B69" t="n">
         <v>333043</v>
@@ -1957,10 +1827,8 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="1" t="inlineStr">
-        <is>
-          <t>2016-09</t>
-        </is>
+      <c r="A70" s="2" t="n">
+        <v>42614</v>
       </c>
       <c r="B70" t="n">
         <v>284954</v>
@@ -1979,10 +1847,8 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="1" t="inlineStr">
-        <is>
-          <t>2016-10</t>
-        </is>
+      <c r="A71" s="2" t="n">
+        <v>42644</v>
       </c>
       <c r="B71" t="n">
         <v>272642</v>
@@ -2001,10 +1867,8 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="1" t="inlineStr">
-        <is>
-          <t>2016-11</t>
-        </is>
+      <c r="A72" s="2" t="n">
+        <v>42675</v>
       </c>
       <c r="B72" t="n">
         <v>192628</v>
@@ -2023,10 +1887,8 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="1" t="inlineStr">
-        <is>
-          <t>2016-12</t>
-        </is>
+      <c r="A73" s="2" t="n">
+        <v>42705</v>
       </c>
       <c r="B73" t="n">
         <v>187820</v>
@@ -2045,10 +1907,8 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="1" t="inlineStr">
-        <is>
-          <t>2017-01</t>
-        </is>
+      <c r="A74" s="2" t="n">
+        <v>42736</v>
       </c>
       <c r="B74" t="n">
         <v>157023</v>
@@ -2067,10 +1927,8 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="1" t="inlineStr">
-        <is>
-          <t>2017-02</t>
-        </is>
+      <c r="A75" s="2" t="n">
+        <v>42767</v>
       </c>
       <c r="B75" t="n">
         <v>171119</v>
@@ -2089,10 +1947,8 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="1" t="inlineStr">
-        <is>
-          <t>2017-03</t>
-        </is>
+      <c r="A76" s="2" t="n">
+        <v>42795</v>
       </c>
       <c r="B76" t="n">
         <v>198093</v>
@@ -2111,10 +1967,8 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="1" t="inlineStr">
-        <is>
-          <t>2017-04</t>
-        </is>
+      <c r="A77" s="2" t="n">
+        <v>42826</v>
       </c>
       <c r="B77" t="n">
         <v>258288</v>
@@ -2133,10 +1987,8 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="1" t="inlineStr">
-        <is>
-          <t>2017-05</t>
-        </is>
+      <c r="A78" s="2" t="n">
+        <v>42856</v>
       </c>
       <c r="B78" t="n">
         <v>268060</v>
@@ -2155,10 +2007,8 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="1" t="inlineStr">
-        <is>
-          <t>2017-06</t>
-        </is>
+      <c r="A79" s="2" t="n">
+        <v>42887</v>
       </c>
       <c r="B79" t="n">
         <v>273479</v>
@@ -2177,10 +2027,8 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="1" t="inlineStr">
-        <is>
-          <t>2017-07</t>
-        </is>
+      <c r="A80" s="2" t="n">
+        <v>42917</v>
       </c>
       <c r="B80" t="n">
         <v>314401</v>
@@ -2199,10 +2047,8 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="1" t="inlineStr">
-        <is>
-          <t>2017-08</t>
-        </is>
+      <c r="A81" s="2" t="n">
+        <v>42948</v>
       </c>
       <c r="B81" t="n">
         <v>331979</v>
@@ -2221,10 +2067,8 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="1" t="inlineStr">
-        <is>
-          <t>2017-09</t>
-        </is>
+      <c r="A82" s="2" t="n">
+        <v>42979</v>
       </c>
       <c r="B82" t="n">
         <v>289395</v>
@@ -2243,10 +2087,8 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="1" t="inlineStr">
-        <is>
-          <t>2017-10</t>
-        </is>
+      <c r="A83" s="2" t="n">
+        <v>43009</v>
       </c>
       <c r="B83" t="n">
         <v>272006</v>
@@ -2265,10 +2107,8 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="1" t="inlineStr">
-        <is>
-          <t>2017-11</t>
-        </is>
+      <c r="A84" s="2" t="n">
+        <v>43040</v>
       </c>
       <c r="B84" t="n">
         <v>213143</v>
@@ -2287,10 +2127,8 @@
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="1" t="inlineStr">
-        <is>
-          <t>2017-12</t>
-        </is>
+      <c r="A85" s="2" t="n">
+        <v>43070</v>
       </c>
       <c r="B85" t="n">
         <v>193507</v>
@@ -2309,10 +2147,8 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="1" t="inlineStr">
-        <is>
-          <t>2018-01</t>
-        </is>
+      <c r="A86" s="2" t="n">
+        <v>43101</v>
       </c>
       <c r="B86" t="n">
         <v>157125</v>
@@ -2331,10 +2167,8 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="1" t="inlineStr">
-        <is>
-          <t>2018-02</t>
-        </is>
+      <c r="A87" s="2" t="n">
+        <v>43132</v>
       </c>
       <c r="B87" t="n">
         <v>169737</v>
@@ -2353,10 +2187,8 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="1" t="inlineStr">
-        <is>
-          <t>2018-03</t>
-        </is>
+      <c r="A88" s="2" t="n">
+        <v>43160</v>
       </c>
       <c r="B88" t="n">
         <v>230273</v>
@@ -2375,10 +2207,8 @@
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="1" t="inlineStr">
-        <is>
-          <t>2018-04</t>
-        </is>
+      <c r="A89" s="2" t="n">
+        <v>43191</v>
       </c>
       <c r="B89" t="n">
         <v>255590</v>
@@ -2397,10 +2227,8 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="1" t="inlineStr">
-        <is>
-          <t>2018-05</t>
-        </is>
+      <c r="A90" s="2" t="n">
+        <v>43221</v>
       </c>
       <c r="B90" t="n">
         <v>286084</v>
@@ -2419,10 +2247,8 @@
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="1" t="inlineStr">
-        <is>
-          <t>2018-06</t>
-        </is>
+      <c r="A91" s="2" t="n">
+        <v>43252</v>
       </c>
       <c r="B91" t="n">
         <v>285853</v>
@@ -2441,10 +2267,8 @@
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="1" t="inlineStr">
-        <is>
-          <t>2018-07</t>
-        </is>
+      <c r="A92" s="2" t="n">
+        <v>43282</v>
       </c>
       <c r="B92" t="n">
         <v>322653</v>
@@ -2463,10 +2287,8 @@
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="1" t="inlineStr">
-        <is>
-          <t>2018-08</t>
-        </is>
+      <c r="A93" s="2" t="n">
+        <v>43313</v>
       </c>
       <c r="B93" t="n">
         <v>354146</v>
@@ -2485,10 +2307,8 @@
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="1" t="inlineStr">
-        <is>
-          <t>2018-09</t>
-        </is>
+      <c r="A94" s="2" t="n">
+        <v>43344</v>
       </c>
       <c r="B94" t="n">
         <v>299174</v>
@@ -2507,10 +2327,8 @@
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="1" t="inlineStr">
-        <is>
-          <t>2018-10</t>
-        </is>
+      <c r="A95" s="2" t="n">
+        <v>43374</v>
       </c>
       <c r="B95" t="n">
         <v>281042</v>
@@ -2529,10 +2347,8 @@
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="1" t="inlineStr">
-        <is>
-          <t>2018-11</t>
-        </is>
+      <c r="A96" s="2" t="n">
+        <v>43405</v>
       </c>
       <c r="B96" t="n">
         <v>225791</v>
@@ -2551,10 +2367,8 @@
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="1" t="inlineStr">
-        <is>
-          <t>2018-12</t>
-        </is>
+      <c r="A97" s="2" t="n">
+        <v>43435</v>
       </c>
       <c r="B97" t="n">
         <v>203662</v>
@@ -2573,10 +2387,8 @@
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="1" t="inlineStr">
-        <is>
-          <t>2019-01</t>
-        </is>
+      <c r="A98" s="2" t="n">
+        <v>43466</v>
       </c>
       <c r="B98" t="n">
         <v>161662</v>
@@ -2595,10 +2407,8 @@
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="1" t="inlineStr">
-        <is>
-          <t>2019-02</t>
-        </is>
+      <c r="A99" s="2" t="n">
+        <v>43497</v>
       </c>
       <c r="B99" t="n">
         <v>179108</v>
@@ -2617,10 +2427,8 @@
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="1" t="inlineStr">
-        <is>
-          <t>2019-03</t>
-        </is>
+      <c r="A100" s="2" t="n">
+        <v>43525</v>
       </c>
       <c r="B100" t="n">
         <v>238822</v>
@@ -2639,10 +2447,8 @@
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="1" t="inlineStr">
-        <is>
-          <t>2019-04</t>
-        </is>
+      <c r="A101" s="2" t="n">
+        <v>43556</v>
       </c>
       <c r="B101" t="n">
         <v>276415</v>
@@ -2661,10 +2467,8 @@
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="1" t="inlineStr">
-        <is>
-          <t>2019-05</t>
-        </is>
+      <c r="A102" s="2" t="n">
+        <v>43586</v>
       </c>
       <c r="B102" t="n">
         <v>295055</v>
@@ -2683,10 +2487,8 @@
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="1" t="inlineStr">
-        <is>
-          <t>2019-06</t>
-        </is>
+      <c r="A103" s="2" t="n">
+        <v>43617</v>
       </c>
       <c r="B103" t="n">
         <v>298247</v>
@@ -2705,10 +2507,8 @@
       </c>
     </row>
     <row r="104">
-      <c r="A104" s="1" t="inlineStr">
-        <is>
-          <t>2019-07</t>
-        </is>
+      <c r="A104" s="2" t="n">
+        <v>43647</v>
       </c>
       <c r="B104" t="n">
         <v>328082</v>
@@ -2727,10 +2527,8 @@
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="1" t="inlineStr">
-        <is>
-          <t>2019-08</t>
-        </is>
+      <c r="A105" s="2" t="n">
+        <v>43678</v>
       </c>
       <c r="B105" t="n">
         <v>357035</v>
@@ -2749,10 +2547,8 @@
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="1" t="inlineStr">
-        <is>
-          <t>2019-09</t>
-        </is>
+      <c r="A106" s="2" t="n">
+        <v>43709</v>
       </c>
       <c r="B106" t="n">
         <v>316931</v>
@@ -2771,10 +2567,8 @@
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="1" t="inlineStr">
-        <is>
-          <t>2019-10</t>
-        </is>
+      <c r="A107" s="2" t="n">
+        <v>43739</v>
       </c>
       <c r="B107" t="n">
         <v>296538</v>
@@ -2793,10 +2587,8 @@
       </c>
     </row>
     <row r="108">
-      <c r="A108" s="1" t="inlineStr">
-        <is>
-          <t>2019-11</t>
-        </is>
+      <c r="A108" s="2" t="n">
+        <v>43770</v>
       </c>
       <c r="B108" t="n">
         <v>228196</v>
@@ -2815,10 +2607,8 @@
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="1" t="inlineStr">
-        <is>
-          <t>2019-12</t>
-        </is>
+      <c r="A109" s="2" t="n">
+        <v>43800</v>
       </c>
       <c r="B109" t="n">
         <v>208813</v>
@@ -2837,10 +2627,8 @@
       </c>
     </row>
     <row r="110">
-      <c r="A110" s="1" t="inlineStr">
-        <is>
-          <t>2020-01</t>
-        </is>
+      <c r="A110" s="2" t="n">
+        <v>43831</v>
       </c>
       <c r="B110" t="n">
         <v>173251</v>
@@ -2859,10 +2647,8 @@
       </c>
     </row>
     <row r="111">
-      <c r="A111" s="1" t="inlineStr">
-        <is>
-          <t>2020-02</t>
-        </is>
+      <c r="A111" s="2" t="n">
+        <v>43862</v>
       </c>
       <c r="B111" t="n">
         <v>206297</v>
@@ -2881,10 +2667,8 @@
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="1" t="inlineStr">
-        <is>
-          <t>2020-03</t>
-        </is>
+      <c r="A112" s="2" t="n">
+        <v>43891</v>
       </c>
       <c r="B112" t="n">
         <v>67544</v>
@@ -2903,706 +2687,602 @@
       </c>
     </row>
     <row r="113">
-      <c r="A113" s="1" t="inlineStr">
-        <is>
-          <t>2020-06</t>
-        </is>
+      <c r="A113" s="2" t="n">
+        <v>44044</v>
       </c>
       <c r="B113" t="n">
-        <v>47669</v>
+        <v>216967</v>
       </c>
       <c r="C113" t="n">
-        <v>31779</v>
+        <v>147203</v>
       </c>
       <c r="D113" t="n">
-        <v>15890</v>
+        <v>69764</v>
       </c>
       <c r="E113" t="n">
-        <v>6355.8</v>
+        <v>29440.6</v>
       </c>
       <c r="F113" t="n">
-        <v>7945</v>
+        <v>34882</v>
       </c>
     </row>
     <row r="114">
-      <c r="A114" s="1" t="inlineStr">
-        <is>
-          <t>2020-07</t>
-        </is>
+      <c r="A114" s="2" t="n">
+        <v>44075</v>
       </c>
       <c r="B114" t="n">
-        <v>179843</v>
+        <v>130004</v>
       </c>
       <c r="C114" t="n">
-        <v>110279</v>
+        <v>80437</v>
       </c>
       <c r="D114" t="n">
-        <v>69564</v>
+        <v>49567</v>
       </c>
       <c r="E114" t="n">
-        <v>22055.8</v>
+        <v>16087.4</v>
       </c>
       <c r="F114" t="n">
-        <v>34782</v>
+        <v>24783.5</v>
       </c>
     </row>
     <row r="115">
-      <c r="A115" s="1" t="inlineStr">
-        <is>
-          <t>2020-08</t>
-        </is>
+      <c r="A115" s="2" t="n">
+        <v>44105</v>
       </c>
       <c r="B115" t="n">
-        <v>216967</v>
+        <v>109393</v>
       </c>
       <c r="C115" t="n">
-        <v>147203</v>
+        <v>60476</v>
       </c>
       <c r="D115" t="n">
-        <v>69764</v>
+        <v>48917</v>
       </c>
       <c r="E115" t="n">
-        <v>29440.6</v>
+        <v>12095.2</v>
       </c>
       <c r="F115" t="n">
-        <v>34882</v>
+        <v>24458.5</v>
       </c>
     </row>
     <row r="116">
-      <c r="A116" s="1" t="inlineStr">
-        <is>
-          <t>2020-09</t>
-        </is>
+      <c r="A116" s="2" t="n">
+        <v>44136</v>
       </c>
       <c r="B116" t="n">
-        <v>130004</v>
+        <v>41367</v>
       </c>
       <c r="C116" t="n">
-        <v>80437</v>
+        <v>29732</v>
       </c>
       <c r="D116" t="n">
-        <v>49567</v>
+        <v>11635</v>
       </c>
       <c r="E116" t="n">
-        <v>16087.4</v>
+        <v>5946.4</v>
       </c>
       <c r="F116" t="n">
-        <v>24783.5</v>
+        <v>5817.5</v>
       </c>
     </row>
     <row r="117">
-      <c r="A117" s="1" t="inlineStr">
-        <is>
-          <t>2020-10</t>
-        </is>
+      <c r="A117" s="2" t="n">
+        <v>44166</v>
       </c>
       <c r="B117" t="n">
-        <v>109393</v>
+        <v>56534</v>
       </c>
       <c r="C117" t="n">
-        <v>60476</v>
+        <v>38205</v>
       </c>
       <c r="D117" t="n">
-        <v>48917</v>
+        <v>18329</v>
       </c>
       <c r="E117" t="n">
-        <v>12095.2</v>
+        <v>7641</v>
       </c>
       <c r="F117" t="n">
-        <v>24458.5</v>
+        <v>9164.5</v>
       </c>
     </row>
     <row r="118">
-      <c r="A118" s="1" t="inlineStr">
-        <is>
-          <t>2020-11</t>
-        </is>
+      <c r="A118" s="2" t="n">
+        <v>44197</v>
       </c>
       <c r="B118" t="n">
-        <v>41367</v>
+        <v>49181</v>
       </c>
       <c r="C118" t="n">
-        <v>29732</v>
+        <v>28304</v>
       </c>
       <c r="D118" t="n">
-        <v>11635</v>
+        <v>20877</v>
       </c>
       <c r="E118" t="n">
-        <v>5946.4</v>
+        <v>5660.8</v>
       </c>
       <c r="F118" t="n">
-        <v>5817.5</v>
+        <v>10438.5</v>
       </c>
     </row>
     <row r="119">
-      <c r="A119" s="1" t="inlineStr">
-        <is>
-          <t>2020-12</t>
-        </is>
+      <c r="A119" s="2" t="n">
+        <v>44228</v>
       </c>
       <c r="B119" t="n">
-        <v>56534</v>
+        <v>48531</v>
       </c>
       <c r="C119" t="n">
-        <v>38205</v>
+        <v>30266</v>
       </c>
       <c r="D119" t="n">
-        <v>18329</v>
+        <v>18265</v>
       </c>
       <c r="E119" t="n">
-        <v>7641</v>
+        <v>6053.2</v>
       </c>
       <c r="F119" t="n">
-        <v>9164.5</v>
+        <v>9132.5</v>
       </c>
     </row>
     <row r="120">
-      <c r="A120" s="1" t="inlineStr">
-        <is>
-          <t>2021-01</t>
-        </is>
+      <c r="A120" s="2" t="n">
+        <v>44256</v>
       </c>
       <c r="B120" t="n">
-        <v>49181</v>
+        <v>89930</v>
       </c>
       <c r="C120" t="n">
-        <v>28304</v>
+        <v>52357</v>
       </c>
       <c r="D120" t="n">
-        <v>20877</v>
+        <v>37573</v>
       </c>
       <c r="E120" t="n">
-        <v>5660.8</v>
+        <v>10471.4</v>
       </c>
       <c r="F120" t="n">
-        <v>10438.5</v>
+        <v>18786.5</v>
       </c>
     </row>
     <row r="121">
-      <c r="A121" s="1" t="inlineStr">
-        <is>
-          <t>2021-02</t>
-        </is>
+      <c r="A121" s="2" t="n">
+        <v>44287</v>
       </c>
       <c r="B121" t="n">
-        <v>48531</v>
+        <v>93844</v>
       </c>
       <c r="C121" t="n">
-        <v>30266</v>
+        <v>59218</v>
       </c>
       <c r="D121" t="n">
-        <v>18265</v>
+        <v>34626</v>
       </c>
       <c r="E121" t="n">
-        <v>6053.2</v>
+        <v>11843.6</v>
       </c>
       <c r="F121" t="n">
-        <v>9132.5</v>
+        <v>17313</v>
       </c>
     </row>
     <row r="122">
-      <c r="A122" s="1" t="inlineStr">
-        <is>
-          <t>2021-03</t>
-        </is>
+      <c r="A122" s="2" t="n">
+        <v>44317</v>
       </c>
       <c r="B122" t="n">
-        <v>89930</v>
+        <v>119312</v>
       </c>
       <c r="C122" t="n">
-        <v>52357</v>
+        <v>67572</v>
       </c>
       <c r="D122" t="n">
-        <v>37573</v>
+        <v>51740</v>
       </c>
       <c r="E122" t="n">
-        <v>10471.4</v>
+        <v>13514.4</v>
       </c>
       <c r="F122" t="n">
-        <v>18786.5</v>
+        <v>25870</v>
       </c>
     </row>
     <row r="123">
-      <c r="A123" s="1" t="inlineStr">
-        <is>
-          <t>2021-04</t>
-        </is>
+      <c r="A123" s="2" t="n">
+        <v>44348</v>
       </c>
       <c r="B123" t="n">
-        <v>93844</v>
+        <v>172095</v>
       </c>
       <c r="C123" t="n">
-        <v>59218</v>
+        <v>106781</v>
       </c>
       <c r="D123" t="n">
-        <v>34626</v>
+        <v>65314</v>
       </c>
       <c r="E123" t="n">
-        <v>11843.6</v>
+        <v>21356.2</v>
       </c>
       <c r="F123" t="n">
-        <v>17313</v>
+        <v>32657</v>
       </c>
     </row>
     <row r="124">
-      <c r="A124" s="1" t="inlineStr">
-        <is>
-          <t>2021-05</t>
-        </is>
+      <c r="A124" s="2" t="n">
+        <v>44378</v>
       </c>
       <c r="B124" t="n">
-        <v>119312</v>
+        <v>292165</v>
       </c>
       <c r="C124" t="n">
-        <v>67572</v>
+        <v>174682</v>
       </c>
       <c r="D124" t="n">
-        <v>51740</v>
+        <v>117483</v>
       </c>
       <c r="E124" t="n">
-        <v>13514.4</v>
+        <v>34936.4</v>
       </c>
       <c r="F124" t="n">
-        <v>25870</v>
+        <v>58741.5</v>
       </c>
     </row>
     <row r="125">
-      <c r="A125" s="1" t="inlineStr">
-        <is>
-          <t>2021-06</t>
-        </is>
+      <c r="A125" s="2" t="n">
+        <v>44409</v>
       </c>
       <c r="B125" t="n">
-        <v>172095</v>
+        <v>357683</v>
       </c>
       <c r="C125" t="n">
-        <v>106781</v>
+        <v>257866</v>
       </c>
       <c r="D125" t="n">
-        <v>65314</v>
+        <v>99817</v>
       </c>
       <c r="E125" t="n">
-        <v>21356.2</v>
+        <v>51573.2</v>
       </c>
       <c r="F125" t="n">
-        <v>32657</v>
+        <v>49908.5</v>
       </c>
     </row>
     <row r="126">
-      <c r="A126" s="1" t="inlineStr">
-        <is>
-          <t>2021-07</t>
-        </is>
+      <c r="A126" s="2" t="n">
+        <v>44440</v>
       </c>
       <c r="B126" t="n">
-        <v>292165</v>
+        <v>269420</v>
       </c>
       <c r="C126" t="n">
-        <v>174682</v>
+        <v>177204</v>
       </c>
       <c r="D126" t="n">
-        <v>117483</v>
+        <v>92216</v>
       </c>
       <c r="E126" t="n">
-        <v>34936.4</v>
+        <v>35440.8</v>
       </c>
       <c r="F126" t="n">
-        <v>58741.5</v>
+        <v>46108</v>
       </c>
     </row>
     <row r="127">
-      <c r="A127" s="1" t="inlineStr">
-        <is>
-          <t>2021-08</t>
-        </is>
+      <c r="A127" s="2" t="n">
+        <v>44470</v>
       </c>
       <c r="B127" t="n">
-        <v>357683</v>
+        <v>286392</v>
       </c>
       <c r="C127" t="n">
-        <v>257866</v>
+        <v>159097</v>
       </c>
       <c r="D127" t="n">
-        <v>99817</v>
+        <v>127295</v>
       </c>
       <c r="E127" t="n">
-        <v>51573.2</v>
+        <v>31819.4</v>
       </c>
       <c r="F127" t="n">
-        <v>49908.5</v>
+        <v>63647.5</v>
       </c>
     </row>
     <row r="128">
-      <c r="A128" s="1" t="inlineStr">
-        <is>
-          <t>2021-09</t>
-        </is>
+      <c r="A128" s="2" t="n">
+        <v>44501</v>
       </c>
       <c r="B128" t="n">
-        <v>269420</v>
+        <v>212538</v>
       </c>
       <c r="C128" t="n">
-        <v>177204</v>
+        <v>128867</v>
       </c>
       <c r="D128" t="n">
-        <v>92216</v>
+        <v>83671</v>
       </c>
       <c r="E128" t="n">
-        <v>35440.8</v>
+        <v>25773.4</v>
       </c>
       <c r="F128" t="n">
-        <v>46108</v>
+        <v>41835.5</v>
       </c>
     </row>
     <row r="129">
-      <c r="A129" s="1" t="inlineStr">
-        <is>
-          <t>2021-10</t>
-        </is>
+      <c r="A129" s="2" t="n">
+        <v>44531</v>
       </c>
       <c r="B129" t="n">
-        <v>286392</v>
+        <v>181836</v>
       </c>
       <c r="C129" t="n">
-        <v>159097</v>
+        <v>110718</v>
       </c>
       <c r="D129" t="n">
-        <v>127295</v>
+        <v>71118</v>
       </c>
       <c r="E129" t="n">
-        <v>31819.4</v>
+        <v>22143.6</v>
       </c>
       <c r="F129" t="n">
-        <v>63647.5</v>
+        <v>35559</v>
       </c>
     </row>
     <row r="130">
-      <c r="A130" s="1" t="inlineStr">
-        <is>
-          <t>2021-11</t>
-        </is>
+      <c r="A130" s="2" t="n">
+        <v>44562</v>
       </c>
       <c r="B130" t="n">
-        <v>212538</v>
+        <v>131984</v>
       </c>
       <c r="C130" t="n">
-        <v>128867</v>
+        <v>76902</v>
       </c>
       <c r="D130" t="n">
-        <v>83671</v>
+        <v>55082</v>
       </c>
       <c r="E130" t="n">
-        <v>25773.4</v>
+        <v>15380.4</v>
       </c>
       <c r="F130" t="n">
-        <v>41835.5</v>
+        <v>27541</v>
       </c>
     </row>
     <row r="131">
-      <c r="A131" s="1" t="inlineStr">
-        <is>
-          <t>2021-12</t>
-        </is>
+      <c r="A131" s="2" t="n">
+        <v>44593</v>
       </c>
       <c r="B131" t="n">
-        <v>181836</v>
+        <v>179635</v>
       </c>
       <c r="C131" t="n">
-        <v>110718</v>
+        <v>99238</v>
       </c>
       <c r="D131" t="n">
-        <v>71118</v>
+        <v>80397</v>
       </c>
       <c r="E131" t="n">
-        <v>22143.6</v>
+        <v>19847.6</v>
       </c>
       <c r="F131" t="n">
-        <v>35559</v>
+        <v>40198.5</v>
       </c>
     </row>
     <row r="132">
-      <c r="A132" s="1" t="inlineStr">
-        <is>
-          <t>2022-01</t>
-        </is>
+      <c r="A132" s="2" t="n">
+        <v>44621</v>
       </c>
       <c r="B132" t="n">
-        <v>131984</v>
+        <v>209119</v>
       </c>
       <c r="C132" t="n">
-        <v>76902</v>
+        <v>124471</v>
       </c>
       <c r="D132" t="n">
-        <v>55082</v>
+        <v>84648</v>
       </c>
       <c r="E132" t="n">
-        <v>15380.4</v>
+        <v>24894.2</v>
       </c>
       <c r="F132" t="n">
-        <v>27541</v>
+        <v>42324</v>
       </c>
     </row>
     <row r="133">
-      <c r="A133" s="1" t="inlineStr">
-        <is>
-          <t>2022-02</t>
-        </is>
+      <c r="A133" s="2" t="n">
+        <v>44652</v>
       </c>
       <c r="B133" t="n">
-        <v>179635</v>
+        <v>288487</v>
       </c>
       <c r="C133" t="n">
-        <v>99238</v>
+        <v>169276</v>
       </c>
       <c r="D133" t="n">
-        <v>80397</v>
+        <v>119211</v>
       </c>
       <c r="E133" t="n">
-        <v>19847.6</v>
+        <v>33855.2</v>
       </c>
       <c r="F133" t="n">
-        <v>40198.5</v>
+        <v>59605.5</v>
       </c>
     </row>
     <row r="134">
-      <c r="A134" s="1" t="inlineStr">
-        <is>
-          <t>2022-03</t>
-        </is>
+      <c r="A134" s="2" t="n">
+        <v>44682</v>
       </c>
       <c r="B134" t="n">
-        <v>209119</v>
+        <v>301976</v>
       </c>
       <c r="C134" t="n">
-        <v>124471</v>
+        <v>196165</v>
       </c>
       <c r="D134" t="n">
-        <v>84648</v>
+        <v>105811</v>
       </c>
       <c r="E134" t="n">
-        <v>24894.2</v>
+        <v>39233</v>
       </c>
       <c r="F134" t="n">
-        <v>42324</v>
+        <v>52905.5</v>
       </c>
     </row>
     <row r="135">
-      <c r="A135" s="1" t="inlineStr">
-        <is>
-          <t>2022-04</t>
-        </is>
+      <c r="A135" s="2" t="n">
+        <v>44713</v>
       </c>
       <c r="B135" t="n">
-        <v>288487</v>
+        <v>309162</v>
       </c>
       <c r="C135" t="n">
-        <v>169276</v>
+        <v>208676</v>
       </c>
       <c r="D135" t="n">
-        <v>119211</v>
+        <v>100486</v>
       </c>
       <c r="E135" t="n">
-        <v>33855.2</v>
+        <v>41735.2</v>
       </c>
       <c r="F135" t="n">
-        <v>59605.5</v>
+        <v>50243</v>
       </c>
     </row>
     <row r="136">
-      <c r="A136" s="1" t="inlineStr">
-        <is>
-          <t>2022-05</t>
-        </is>
+      <c r="A136" s="2" t="n">
+        <v>44743</v>
       </c>
       <c r="B136" t="n">
-        <v>301976</v>
+        <v>383186</v>
       </c>
       <c r="C136" t="n">
-        <v>196165</v>
+        <v>242380</v>
       </c>
       <c r="D136" t="n">
-        <v>105811</v>
+        <v>140806</v>
       </c>
       <c r="E136" t="n">
-        <v>39233</v>
+        <v>48476</v>
       </c>
       <c r="F136" t="n">
-        <v>52905.5</v>
+        <v>70403</v>
       </c>
     </row>
     <row r="137">
-      <c r="A137" s="1" t="inlineStr">
-        <is>
-          <t>2022-06</t>
-        </is>
+      <c r="A137" s="2" t="n">
+        <v>44774</v>
       </c>
       <c r="B137" t="n">
-        <v>309162</v>
+        <v>397611</v>
       </c>
       <c r="C137" t="n">
-        <v>208676</v>
+        <v>287565</v>
       </c>
       <c r="D137" t="n">
-        <v>100486</v>
+        <v>110046</v>
       </c>
       <c r="E137" t="n">
-        <v>41735.2</v>
+        <v>57513</v>
       </c>
       <c r="F137" t="n">
-        <v>50243</v>
+        <v>55023</v>
       </c>
     </row>
     <row r="138">
-      <c r="A138" s="1" t="inlineStr">
-        <is>
-          <t>2022-07</t>
-        </is>
+      <c r="A138" s="2" t="n">
+        <v>44805</v>
       </c>
       <c r="B138" t="n">
-        <v>383186</v>
+        <v>330304</v>
       </c>
       <c r="C138" t="n">
-        <v>242380</v>
+        <v>212065</v>
       </c>
       <c r="D138" t="n">
-        <v>140806</v>
+        <v>118239</v>
       </c>
       <c r="E138" t="n">
-        <v>48476</v>
+        <v>42413</v>
       </c>
       <c r="F138" t="n">
-        <v>70403</v>
+        <v>59119.5</v>
       </c>
     </row>
     <row r="139">
-      <c r="A139" s="1" t="inlineStr">
-        <is>
-          <t>2022-08</t>
-        </is>
+      <c r="A139" s="2" t="n">
+        <v>44835</v>
       </c>
       <c r="B139" t="n">
-        <v>397611</v>
+        <v>322320</v>
       </c>
       <c r="C139" t="n">
-        <v>287565</v>
+        <v>200471</v>
       </c>
       <c r="D139" t="n">
-        <v>110046</v>
+        <v>121849</v>
       </c>
       <c r="E139" t="n">
-        <v>57513</v>
+        <v>40094.2</v>
       </c>
       <c r="F139" t="n">
-        <v>55023</v>
+        <v>60924.5</v>
       </c>
     </row>
     <row r="140">
-      <c r="A140" s="1" t="inlineStr">
-        <is>
-          <t>2022-09</t>
-        </is>
+      <c r="A140" s="2" t="n">
+        <v>44866</v>
       </c>
       <c r="B140" t="n">
-        <v>330304</v>
+        <v>247036</v>
       </c>
       <c r="C140" t="n">
-        <v>212065</v>
+        <v>150254</v>
       </c>
       <c r="D140" t="n">
-        <v>118239</v>
+        <v>96782</v>
       </c>
       <c r="E140" t="n">
-        <v>42413</v>
+        <v>30050.8</v>
       </c>
       <c r="F140" t="n">
-        <v>59119.5</v>
+        <v>48391</v>
       </c>
     </row>
     <row r="141">
-      <c r="A141" s="1" t="inlineStr">
-        <is>
-          <t>2022-10</t>
-        </is>
+      <c r="A141" s="2" t="n">
+        <v>44896</v>
       </c>
       <c r="B141" t="n">
-        <v>322320</v>
+        <v>239673</v>
       </c>
       <c r="C141" t="n">
-        <v>200471</v>
+        <v>144684</v>
       </c>
       <c r="D141" t="n">
-        <v>121849</v>
+        <v>94989</v>
       </c>
       <c r="E141" t="n">
-        <v>40094.2</v>
+        <v>28936.8</v>
       </c>
       <c r="F141" t="n">
-        <v>60924.5</v>
+        <v>47494.5</v>
       </c>
     </row>
     <row r="142">
-      <c r="A142" s="1" t="inlineStr">
-        <is>
-          <t>2022-11</t>
-        </is>
+      <c r="A142" s="2" t="n">
+        <v>44927</v>
       </c>
       <c r="B142" t="n">
-        <v>247036</v>
+        <v>191439</v>
       </c>
       <c r="C142" t="n">
-        <v>150254</v>
+        <v>122187</v>
       </c>
       <c r="D142" t="n">
-        <v>96782</v>
+        <v>69252</v>
       </c>
       <c r="E142" t="n">
-        <v>30050.8</v>
+        <v>24437.4</v>
       </c>
       <c r="F142" t="n">
-        <v>48391</v>
-      </c>
-    </row>
-    <row r="143">
-      <c r="A143" s="1" t="inlineStr">
-        <is>
-          <t>2022-12</t>
-        </is>
-      </c>
-      <c r="B143" t="n">
-        <v>239673</v>
-      </c>
-      <c r="C143" t="n">
-        <v>144684</v>
-      </c>
-      <c r="D143" t="n">
-        <v>94989</v>
-      </c>
-      <c r="E143" t="n">
-        <v>28936.8</v>
-      </c>
-      <c r="F143" t="n">
-        <v>47494.5</v>
-      </c>
-    </row>
-    <row r="144">
-      <c r="A144" s="1" t="inlineStr">
-        <is>
-          <t>2023-01</t>
-        </is>
-      </c>
-      <c r="B144" t="n">
-        <v>191439</v>
-      </c>
-      <c r="C144" t="n">
-        <v>122187</v>
-      </c>
-      <c r="D144" t="n">
-        <v>69252</v>
-      </c>
-      <c r="E144" t="n">
-        <v>24437.4</v>
-      </c>
-      <c r="F144" t="n">
         <v>34626</v>
       </c>
     </row>

</xml_diff>

<commit_message>
entras,pernoctacion por temporada excel
</commit_message>
<xml_diff>
--- a/EDA/DF_DV/Pernoctaciones por dias.xlsx
+++ b/EDA/DF_DV/Pernoctaciones por dias.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F142"/>
+  <dimension ref="A1:F144"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2688,601 +2688,641 @@
     </row>
     <row r="113">
       <c r="A113" s="2" t="n">
-        <v>44044</v>
+        <v>43983</v>
       </c>
       <c r="B113" t="n">
-        <v>216967</v>
+        <v>47669</v>
       </c>
       <c r="C113" t="n">
-        <v>147203</v>
+        <v>31779</v>
       </c>
       <c r="D113" t="n">
-        <v>69764</v>
+        <v>15890</v>
       </c>
       <c r="E113" t="n">
-        <v>29440.6</v>
+        <v>6355.8</v>
       </c>
       <c r="F113" t="n">
-        <v>34882</v>
+        <v>7945</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="2" t="n">
-        <v>44075</v>
+        <v>44013</v>
       </c>
       <c r="B114" t="n">
-        <v>130004</v>
+        <v>179843</v>
       </c>
       <c r="C114" t="n">
-        <v>80437</v>
+        <v>110279</v>
       </c>
       <c r="D114" t="n">
-        <v>49567</v>
+        <v>69564</v>
       </c>
       <c r="E114" t="n">
-        <v>16087.4</v>
+        <v>22055.8</v>
       </c>
       <c r="F114" t="n">
-        <v>24783.5</v>
+        <v>34782</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="2" t="n">
-        <v>44105</v>
+        <v>44044</v>
       </c>
       <c r="B115" t="n">
-        <v>109393</v>
+        <v>216967</v>
       </c>
       <c r="C115" t="n">
-        <v>60476</v>
+        <v>147203</v>
       </c>
       <c r="D115" t="n">
-        <v>48917</v>
+        <v>69764</v>
       </c>
       <c r="E115" t="n">
-        <v>12095.2</v>
+        <v>29440.6</v>
       </c>
       <c r="F115" t="n">
-        <v>24458.5</v>
+        <v>34882</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="2" t="n">
-        <v>44136</v>
+        <v>44075</v>
       </c>
       <c r="B116" t="n">
-        <v>41367</v>
+        <v>130004</v>
       </c>
       <c r="C116" t="n">
-        <v>29732</v>
+        <v>80437</v>
       </c>
       <c r="D116" t="n">
-        <v>11635</v>
+        <v>49567</v>
       </c>
       <c r="E116" t="n">
-        <v>5946.4</v>
+        <v>16087.4</v>
       </c>
       <c r="F116" t="n">
-        <v>5817.5</v>
+        <v>24783.5</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="2" t="n">
-        <v>44166</v>
+        <v>44105</v>
       </c>
       <c r="B117" t="n">
-        <v>56534</v>
+        <v>109393</v>
       </c>
       <c r="C117" t="n">
-        <v>38205</v>
+        <v>60476</v>
       </c>
       <c r="D117" t="n">
-        <v>18329</v>
+        <v>48917</v>
       </c>
       <c r="E117" t="n">
-        <v>7641</v>
+        <v>12095.2</v>
       </c>
       <c r="F117" t="n">
-        <v>9164.5</v>
+        <v>24458.5</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="2" t="n">
-        <v>44197</v>
+        <v>44136</v>
       </c>
       <c r="B118" t="n">
-        <v>49181</v>
+        <v>41367</v>
       </c>
       <c r="C118" t="n">
-        <v>28304</v>
+        <v>29732</v>
       </c>
       <c r="D118" t="n">
-        <v>20877</v>
+        <v>11635</v>
       </c>
       <c r="E118" t="n">
-        <v>5660.8</v>
+        <v>5946.4</v>
       </c>
       <c r="F118" t="n">
-        <v>10438.5</v>
+        <v>5817.5</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="2" t="n">
-        <v>44228</v>
+        <v>44166</v>
       </c>
       <c r="B119" t="n">
-        <v>48531</v>
+        <v>56534</v>
       </c>
       <c r="C119" t="n">
-        <v>30266</v>
+        <v>38205</v>
       </c>
       <c r="D119" t="n">
-        <v>18265</v>
+        <v>18329</v>
       </c>
       <c r="E119" t="n">
-        <v>6053.2</v>
+        <v>7641</v>
       </c>
       <c r="F119" t="n">
-        <v>9132.5</v>
+        <v>9164.5</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="2" t="n">
-        <v>44256</v>
+        <v>44197</v>
       </c>
       <c r="B120" t="n">
-        <v>89930</v>
+        <v>49181</v>
       </c>
       <c r="C120" t="n">
-        <v>52357</v>
+        <v>28304</v>
       </c>
       <c r="D120" t="n">
-        <v>37573</v>
+        <v>20877</v>
       </c>
       <c r="E120" t="n">
-        <v>10471.4</v>
+        <v>5660.8</v>
       </c>
       <c r="F120" t="n">
-        <v>18786.5</v>
+        <v>10438.5</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="2" t="n">
-        <v>44287</v>
+        <v>44228</v>
       </c>
       <c r="B121" t="n">
-        <v>93844</v>
+        <v>48531</v>
       </c>
       <c r="C121" t="n">
-        <v>59218</v>
+        <v>30266</v>
       </c>
       <c r="D121" t="n">
-        <v>34626</v>
+        <v>18265</v>
       </c>
       <c r="E121" t="n">
-        <v>11843.6</v>
+        <v>6053.2</v>
       </c>
       <c r="F121" t="n">
-        <v>17313</v>
+        <v>9132.5</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="2" t="n">
-        <v>44317</v>
+        <v>44256</v>
       </c>
       <c r="B122" t="n">
-        <v>119312</v>
+        <v>89930</v>
       </c>
       <c r="C122" t="n">
-        <v>67572</v>
+        <v>52357</v>
       </c>
       <c r="D122" t="n">
-        <v>51740</v>
+        <v>37573</v>
       </c>
       <c r="E122" t="n">
-        <v>13514.4</v>
+        <v>10471.4</v>
       </c>
       <c r="F122" t="n">
-        <v>25870</v>
+        <v>18786.5</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="2" t="n">
-        <v>44348</v>
+        <v>44287</v>
       </c>
       <c r="B123" t="n">
-        <v>172095</v>
+        <v>93844</v>
       </c>
       <c r="C123" t="n">
-        <v>106781</v>
+        <v>59218</v>
       </c>
       <c r="D123" t="n">
-        <v>65314</v>
+        <v>34626</v>
       </c>
       <c r="E123" t="n">
-        <v>21356.2</v>
+        <v>11843.6</v>
       </c>
       <c r="F123" t="n">
-        <v>32657</v>
+        <v>17313</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="2" t="n">
-        <v>44378</v>
+        <v>44317</v>
       </c>
       <c r="B124" t="n">
-        <v>292165</v>
+        <v>119312</v>
       </c>
       <c r="C124" t="n">
-        <v>174682</v>
+        <v>67572</v>
       </c>
       <c r="D124" t="n">
-        <v>117483</v>
+        <v>51740</v>
       </c>
       <c r="E124" t="n">
-        <v>34936.4</v>
+        <v>13514.4</v>
       </c>
       <c r="F124" t="n">
-        <v>58741.5</v>
+        <v>25870</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="2" t="n">
-        <v>44409</v>
+        <v>44348</v>
       </c>
       <c r="B125" t="n">
-        <v>357683</v>
+        <v>172095</v>
       </c>
       <c r="C125" t="n">
-        <v>257866</v>
+        <v>106781</v>
       </c>
       <c r="D125" t="n">
-        <v>99817</v>
+        <v>65314</v>
       </c>
       <c r="E125" t="n">
-        <v>51573.2</v>
+        <v>21356.2</v>
       </c>
       <c r="F125" t="n">
-        <v>49908.5</v>
+        <v>32657</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="2" t="n">
-        <v>44440</v>
+        <v>44378</v>
       </c>
       <c r="B126" t="n">
-        <v>269420</v>
+        <v>292165</v>
       </c>
       <c r="C126" t="n">
-        <v>177204</v>
+        <v>174682</v>
       </c>
       <c r="D126" t="n">
-        <v>92216</v>
+        <v>117483</v>
       </c>
       <c r="E126" t="n">
-        <v>35440.8</v>
+        <v>34936.4</v>
       </c>
       <c r="F126" t="n">
-        <v>46108</v>
+        <v>58741.5</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="2" t="n">
-        <v>44470</v>
+        <v>44409</v>
       </c>
       <c r="B127" t="n">
-        <v>286392</v>
+        <v>357683</v>
       </c>
       <c r="C127" t="n">
-        <v>159097</v>
+        <v>257866</v>
       </c>
       <c r="D127" t="n">
-        <v>127295</v>
+        <v>99817</v>
       </c>
       <c r="E127" t="n">
-        <v>31819.4</v>
+        <v>51573.2</v>
       </c>
       <c r="F127" t="n">
-        <v>63647.5</v>
+        <v>49908.5</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="2" t="n">
-        <v>44501</v>
+        <v>44440</v>
       </c>
       <c r="B128" t="n">
-        <v>212538</v>
+        <v>269420</v>
       </c>
       <c r="C128" t="n">
-        <v>128867</v>
+        <v>177204</v>
       </c>
       <c r="D128" t="n">
-        <v>83671</v>
+        <v>92216</v>
       </c>
       <c r="E128" t="n">
-        <v>25773.4</v>
+        <v>35440.8</v>
       </c>
       <c r="F128" t="n">
-        <v>41835.5</v>
+        <v>46108</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="2" t="n">
-        <v>44531</v>
+        <v>44470</v>
       </c>
       <c r="B129" t="n">
-        <v>181836</v>
+        <v>286392</v>
       </c>
       <c r="C129" t="n">
-        <v>110718</v>
+        <v>159097</v>
       </c>
       <c r="D129" t="n">
-        <v>71118</v>
+        <v>127295</v>
       </c>
       <c r="E129" t="n">
-        <v>22143.6</v>
+        <v>31819.4</v>
       </c>
       <c r="F129" t="n">
-        <v>35559</v>
+        <v>63647.5</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="2" t="n">
-        <v>44562</v>
+        <v>44501</v>
       </c>
       <c r="B130" t="n">
-        <v>131984</v>
+        <v>212538</v>
       </c>
       <c r="C130" t="n">
-        <v>76902</v>
+        <v>128867</v>
       </c>
       <c r="D130" t="n">
-        <v>55082</v>
+        <v>83671</v>
       </c>
       <c r="E130" t="n">
-        <v>15380.4</v>
+        <v>25773.4</v>
       </c>
       <c r="F130" t="n">
-        <v>27541</v>
+        <v>41835.5</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="2" t="n">
-        <v>44593</v>
+        <v>44531</v>
       </c>
       <c r="B131" t="n">
-        <v>179635</v>
+        <v>181836</v>
       </c>
       <c r="C131" t="n">
-        <v>99238</v>
+        <v>110718</v>
       </c>
       <c r="D131" t="n">
-        <v>80397</v>
+        <v>71118</v>
       </c>
       <c r="E131" t="n">
-        <v>19847.6</v>
+        <v>22143.6</v>
       </c>
       <c r="F131" t="n">
-        <v>40198.5</v>
+        <v>35559</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="2" t="n">
-        <v>44621</v>
+        <v>44562</v>
       </c>
       <c r="B132" t="n">
-        <v>209119</v>
+        <v>131984</v>
       </c>
       <c r="C132" t="n">
-        <v>124471</v>
+        <v>76902</v>
       </c>
       <c r="D132" t="n">
-        <v>84648</v>
+        <v>55082</v>
       </c>
       <c r="E132" t="n">
-        <v>24894.2</v>
+        <v>15380.4</v>
       </c>
       <c r="F132" t="n">
-        <v>42324</v>
+        <v>27541</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="2" t="n">
-        <v>44652</v>
+        <v>44593</v>
       </c>
       <c r="B133" t="n">
-        <v>288487</v>
+        <v>179635</v>
       </c>
       <c r="C133" t="n">
-        <v>169276</v>
+        <v>99238</v>
       </c>
       <c r="D133" t="n">
-        <v>119211</v>
+        <v>80397</v>
       </c>
       <c r="E133" t="n">
-        <v>33855.2</v>
+        <v>19847.6</v>
       </c>
       <c r="F133" t="n">
-        <v>59605.5</v>
+        <v>40198.5</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="2" t="n">
-        <v>44682</v>
+        <v>44621</v>
       </c>
       <c r="B134" t="n">
-        <v>301976</v>
+        <v>209119</v>
       </c>
       <c r="C134" t="n">
-        <v>196165</v>
+        <v>124471</v>
       </c>
       <c r="D134" t="n">
-        <v>105811</v>
+        <v>84648</v>
       </c>
       <c r="E134" t="n">
-        <v>39233</v>
+        <v>24894.2</v>
       </c>
       <c r="F134" t="n">
-        <v>52905.5</v>
+        <v>42324</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="2" t="n">
-        <v>44713</v>
+        <v>44652</v>
       </c>
       <c r="B135" t="n">
-        <v>309162</v>
+        <v>288487</v>
       </c>
       <c r="C135" t="n">
-        <v>208676</v>
+        <v>169276</v>
       </c>
       <c r="D135" t="n">
-        <v>100486</v>
+        <v>119211</v>
       </c>
       <c r="E135" t="n">
-        <v>41735.2</v>
+        <v>33855.2</v>
       </c>
       <c r="F135" t="n">
-        <v>50243</v>
+        <v>59605.5</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="2" t="n">
-        <v>44743</v>
+        <v>44682</v>
       </c>
       <c r="B136" t="n">
-        <v>383186</v>
+        <v>301976</v>
       </c>
       <c r="C136" t="n">
-        <v>242380</v>
+        <v>196165</v>
       </c>
       <c r="D136" t="n">
-        <v>140806</v>
+        <v>105811</v>
       </c>
       <c r="E136" t="n">
-        <v>48476</v>
+        <v>39233</v>
       </c>
       <c r="F136" t="n">
-        <v>70403</v>
+        <v>52905.5</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="2" t="n">
-        <v>44774</v>
+        <v>44713</v>
       </c>
       <c r="B137" t="n">
-        <v>397611</v>
+        <v>309162</v>
       </c>
       <c r="C137" t="n">
-        <v>287565</v>
+        <v>208676</v>
       </c>
       <c r="D137" t="n">
-        <v>110046</v>
+        <v>100486</v>
       </c>
       <c r="E137" t="n">
-        <v>57513</v>
+        <v>41735.2</v>
       </c>
       <c r="F137" t="n">
-        <v>55023</v>
+        <v>50243</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="2" t="n">
-        <v>44805</v>
+        <v>44743</v>
       </c>
       <c r="B138" t="n">
-        <v>330304</v>
+        <v>383186</v>
       </c>
       <c r="C138" t="n">
-        <v>212065</v>
+        <v>242380</v>
       </c>
       <c r="D138" t="n">
-        <v>118239</v>
+        <v>140806</v>
       </c>
       <c r="E138" t="n">
-        <v>42413</v>
+        <v>48476</v>
       </c>
       <c r="F138" t="n">
-        <v>59119.5</v>
+        <v>70403</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="2" t="n">
-        <v>44835</v>
+        <v>44774</v>
       </c>
       <c r="B139" t="n">
-        <v>322320</v>
+        <v>397611</v>
       </c>
       <c r="C139" t="n">
-        <v>200471</v>
+        <v>287565</v>
       </c>
       <c r="D139" t="n">
-        <v>121849</v>
+        <v>110046</v>
       </c>
       <c r="E139" t="n">
-        <v>40094.2</v>
+        <v>57513</v>
       </c>
       <c r="F139" t="n">
-        <v>60924.5</v>
+        <v>55023</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="2" t="n">
-        <v>44866</v>
+        <v>44805</v>
       </c>
       <c r="B140" t="n">
-        <v>247036</v>
+        <v>330304</v>
       </c>
       <c r="C140" t="n">
-        <v>150254</v>
+        <v>212065</v>
       </c>
       <c r="D140" t="n">
-        <v>96782</v>
+        <v>118239</v>
       </c>
       <c r="E140" t="n">
-        <v>30050.8</v>
+        <v>42413</v>
       </c>
       <c r="F140" t="n">
-        <v>48391</v>
+        <v>59119.5</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="2" t="n">
-        <v>44896</v>
+        <v>44835</v>
       </c>
       <c r="B141" t="n">
-        <v>239673</v>
+        <v>322320</v>
       </c>
       <c r="C141" t="n">
-        <v>144684</v>
+        <v>200471</v>
       </c>
       <c r="D141" t="n">
-        <v>94989</v>
+        <v>121849</v>
       </c>
       <c r="E141" t="n">
-        <v>28936.8</v>
+        <v>40094.2</v>
       </c>
       <c r="F141" t="n">
-        <v>47494.5</v>
+        <v>60924.5</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="2" t="n">
+        <v>44866</v>
+      </c>
+      <c r="B142" t="n">
+        <v>247036</v>
+      </c>
+      <c r="C142" t="n">
+        <v>150254</v>
+      </c>
+      <c r="D142" t="n">
+        <v>96782</v>
+      </c>
+      <c r="E142" t="n">
+        <v>30050.8</v>
+      </c>
+      <c r="F142" t="n">
+        <v>48391</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="2" t="n">
+        <v>44896</v>
+      </c>
+      <c r="B143" t="n">
+        <v>239673</v>
+      </c>
+      <c r="C143" t="n">
+        <v>144684</v>
+      </c>
+      <c r="D143" t="n">
+        <v>94989</v>
+      </c>
+      <c r="E143" t="n">
+        <v>28936.8</v>
+      </c>
+      <c r="F143" t="n">
+        <v>47494.5</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="2" t="n">
         <v>44927</v>
       </c>
-      <c r="B142" t="n">
+      <c r="B144" t="n">
         <v>191439</v>
       </c>
-      <c r="C142" t="n">
+      <c r="C144" t="n">
         <v>122187</v>
       </c>
-      <c r="D142" t="n">
+      <c r="D144" t="n">
         <v>69252</v>
       </c>
-      <c r="E142" t="n">
+      <c r="E144" t="n">
         <v>24437.4</v>
       </c>
-      <c r="F142" t="n">
+      <c r="F144" t="n">
         <v>34626</v>
       </c>
     </row>

</xml_diff>